<commit_message>
Added info about jumpers and updated BOM.
</commit_message>
<xml_diff>
--- a/IO-module/hardware/IO-module-V1.2-BOM_bot.xlsx
+++ b/IO-module/hardware/IO-module-V1.2-BOM_bot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabfa\Nextcloud2\Bastel-Projekte\Feudal Tech\Offizielles\OpenDINRail\IO-module\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Nextcloud\Bastel-Projekte\Feudal Tech\Offizielles\OpenDINRail\IO-module\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2E13CF-413A-4EC5-938F-7D1B97003DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5591EBA-9CE9-425A-B175-6AF4F60DFA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="4500" windowWidth="28800" windowHeight="15345" xr2:uid="{C36FB6B4-5DEC-4052-8013-72AFCEEE5561}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C36FB6B4-5DEC-4052-8013-72AFCEEE5561}"/>
   </bookViews>
   <sheets>
     <sheet name="Trebuchet-V1-BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="72">
   <si>
     <t>Id</t>
   </si>
@@ -88,9 +88,6 @@
     <t>SOP-16_4.4x10.4mm_P1.27mm</t>
   </si>
   <si>
-    <t>TCMT4100</t>
-  </si>
-  <si>
     <t>R18,R17</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Make sure to use terminals with 5mm spacing not 5.08mm! Does not need to be 10 at one piece. Combining multiple to add to 10 will be fine</t>
-  </si>
-  <si>
     <t>https://de.aliexpress.com/item/32892759207.html</t>
   </si>
   <si>
@@ -197,6 +191,51 @@
   </si>
   <si>
     <t>Through hole parts. (Need to be soldered by yourself)</t>
+  </si>
+  <si>
+    <t>LCSC Number</t>
+  </si>
+  <si>
+    <t>C129022</t>
+  </si>
+  <si>
+    <t>C21190</t>
+  </si>
+  <si>
+    <t>C22962</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C845537</t>
+  </si>
+  <si>
+    <t>C112623</t>
+  </si>
+  <si>
+    <t>TLP293-4</t>
+  </si>
+  <si>
+    <t>C23212</t>
+  </si>
+  <si>
+    <t>C506653</t>
+  </si>
+  <si>
+    <t>C2897391</t>
+  </si>
+  <si>
+    <t>C8404</t>
+  </si>
+  <si>
+    <t>Make sure to use terminals with 5mm spacing not 5.08mm! Does not need to be 10 at one piece. Combining multiple to add to 10 will be fine. (LSCS number is only 2 so 5 need to be connected together)</t>
+  </si>
+  <si>
+    <t>C2894966</t>
   </si>
 </sst>
 </file>
@@ -1082,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C2EAD2-2B23-44A8-A12E-E96D1D8EAAFC}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1100,7 +1139,7 @@
     <col min="9" max="9" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1117,19 +1156,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
+      <c r="J1" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1145,8 +1187,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1163,19 +1208,22 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>54</v>
+      <c r="J3" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1191,8 +1239,11 @@
       <c r="E4">
         <v>220</v>
       </c>
+      <c r="J4" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1208,8 +1259,11 @@
       <c r="E5" t="s">
         <v>14</v>
       </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1225,8 +1279,11 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1242,8 +1299,11 @@
       <c r="E7" t="s">
         <v>19</v>
       </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1257,15 +1317,18 @@
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>65</v>
+      </c>
+      <c r="J8" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1274,15 +1337,15 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -1291,128 +1354,143 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D11" s="2">
         <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>57</v>
+      <c r="J11" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D12" s="2">
         <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>51</v>
+      <c r="J12" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="J13" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D14" s="2">
         <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="I14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>48</v>
+      <c r="J14" t="s">
+        <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
       </c>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>